<commit_message>
QuestManager and QuestInfo which are not tested yet
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterQuest.xlsx
+++ b/Assets/Data/Excel/MasterQuest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A974A37A-8648-435E-8983-71381C0C59DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C20B6C6-AA73-4733-B643-A8A3703ACAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>id</t>
   </si>
@@ -49,30 +49,12 @@
     <t>prerequisiteKey</t>
   </si>
   <si>
-    <t>description01</t>
-  </si>
-  <si>
     <t>Call my father?</t>
   </si>
   <si>
     <t>An unknown presence..</t>
   </si>
   <si>
-    <t>rewardKey</t>
-  </si>
-  <si>
-    <t>rewardAmount</t>
-  </si>
-  <si>
-    <t>actionType01</t>
-  </si>
-  <si>
-    <t>requiredAmount01</t>
-  </si>
-  <si>
-    <t>isDisplayQuest</t>
-  </si>
-  <si>
     <t>Scavenge for coins.</t>
   </si>
   <si>
@@ -82,47 +64,104 @@
     <t>rewardKey that is empty adds toward story progression.</t>
   </si>
   <si>
-    <t>objectiveKey01</t>
-  </si>
-  <si>
-    <t>description02</t>
-  </si>
-  <si>
-    <t>actionType02</t>
-  </si>
-  <si>
-    <t>objectiveKey02</t>
-  </si>
-  <si>
     <t>DialogueResponse</t>
   </si>
   <si>
     <t>Acquire</t>
   </si>
   <si>
-    <t>ActionType</t>
-  </si>
-  <si>
-    <t>DialogueResponse, The dialogue response answer</t>
-  </si>
-  <si>
-    <t>Kill, Eliminate enemy</t>
-  </si>
-  <si>
-    <t>Acquire, Get item</t>
-  </si>
-  <si>
-    <t>Interact, Talk/Examine an people/object</t>
-  </si>
-  <si>
-    <t>ReachArea, Reach a place</t>
+    <t>isHiddenQuest</t>
+  </si>
+  <si>
+    <t>taskDescription01</t>
+  </si>
+  <si>
+    <t>taskActionType01</t>
+  </si>
+  <si>
+    <t>taskObjectiveKey01</t>
+  </si>
+  <si>
+    <t>taskRequiredAmount01</t>
+  </si>
+  <si>
+    <t>taskDescription02</t>
+  </si>
+  <si>
+    <t>taskActionType02</t>
+  </si>
+  <si>
+    <t>taskObjectiveKey02</t>
+  </si>
+  <si>
+    <t>taskRequiredAmount02</t>
+  </si>
+  <si>
+    <t>taskDescription03</t>
+  </si>
+  <si>
+    <t>taskActionType03</t>
+  </si>
+  <si>
+    <t>taskObjectiveKey03</t>
+  </si>
+  <si>
+    <t>taskRequiredAmount03</t>
+  </si>
+  <si>
+    <t>taskActionType of DialogueResponse need to fill in dialogue id into taskObjectiveKey</t>
+  </si>
+  <si>
+    <t>rewardAmount03</t>
+  </si>
+  <si>
+    <t>rewardKey03</t>
+  </si>
+  <si>
+    <t>rewardAmount02</t>
+  </si>
+  <si>
+    <t>rewardKey02</t>
+  </si>
+  <si>
+    <t>rewardAmount01</t>
+  </si>
+  <si>
+    <t>rewardKey01</t>
+  </si>
+  <si>
+    <t>Purchase Amulet from the vending machine</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>Green is main quest. Orange is sub quest</t>
+  </si>
+  <si>
+    <t>None = 0,</t>
+  </si>
+  <si>
+    <t>DialogueResponse,</t>
+  </si>
+  <si>
+    <t>Kill,</t>
+  </si>
+  <si>
+    <t>Acquire,</t>
+  </si>
+  <si>
+    <t>Use,</t>
+  </si>
+  <si>
+    <t>Interact,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,8 +176,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,8 +203,18 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -174,16 +237,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
@@ -500,7 +585,7 @@
   <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,17 +593,27 @@
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="47.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="70.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
@@ -538,97 +633,140 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="H2" s="3">
+        <v>2</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>25000</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>20000</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>20000</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
+      <c r="H3" s="2">
+        <v>10304</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="2">
+        <v>10304</v>
+      </c>
+      <c r="M3" s="2">
+        <v>2</v>
+      </c>
+      <c r="S3" s="2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>20001</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>20000</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3">
-        <v>10304</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
+      <c r="Y3" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -642,39 +780,39 @@
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>22</v>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>23</v>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>24</v>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>25</v>
+      <c r="B6" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>26</v>
+      <c r="B7" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to initialize quest + GlossaryManager + QuestData + Fixed previous changed enum for prefabs
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterQuest.xlsx
+++ b/Assets/Data/Excel/MasterQuest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C20B6C6-AA73-4733-B643-A8A3703ACAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2C7C2F-5899-44EC-A5D7-E575C96CDFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -161,7 +161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,20 +178,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,11 +194,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -253,22 +241,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
+  <cellStyles count="3">
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
@@ -585,7 +569,7 @@
   <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,35 +674,35 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+    <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>20000</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>2</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="2">
         <v>1</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Quest reward to story points + slide animation when quest appears/disappears
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterQuest.xlsx
+++ b/Assets/Data/Excel/MasterQuest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FE97BE-DBB6-4F52-B74D-DD402DF6AE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA2C3A6-5E12-457D-AC12-2246006EEF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Economic hardship</t>
   </si>
   <si>
-    <t>rewardKey that is empty adds toward story progression.</t>
-  </si>
-  <si>
     <t>DialogueResponse</t>
   </si>
   <si>
@@ -151,10 +148,10 @@
     <t>Interact,</t>
   </si>
   <si>
-    <t>taskActionType of DialogueResponse need to fill in dialogue id into taskObjectiveKey.</t>
-  </si>
-  <si>
-    <t>fill in the answer in taskRequiredAmount.</t>
+    <t>rewardKey &lt; 0 add towards story progression. Empty rewardKey gives nothing.</t>
+  </si>
+  <si>
+    <t>taskActionType of DialogueResponse, you need to fill in dialogue id into taskObjectiveKey. Fill in the response answer in taskRequiredAmount.</t>
   </si>
 </sst>
 </file>
@@ -567,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,7 +581,7 @@
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.21875" bestFit="1" customWidth="1"/>
@@ -592,13 +589,13 @@
     <col min="15" max="15" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="70.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="118" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
@@ -612,64 +609,64 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" t="s">
         <v>23</v>
-      </c>
-      <c r="R1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" t="s">
-        <v>24</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>38</v>
@@ -692,7 +689,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" s="2">
         <v>2</v>
@@ -700,11 +697,14 @@
       <c r="I2" s="2">
         <v>0</v>
       </c>
+      <c r="R2" s="2">
+        <v>-1</v>
+      </c>
       <c r="S2" s="2">
         <v>1</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -727,7 +727,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="2">
         <v>10304</v>
@@ -736,10 +736,10 @@
         <v>2</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="L3" s="2">
         <v>10304</v>
@@ -747,14 +747,11 @@
       <c r="M3" s="2">
         <v>2</v>
       </c>
+      <c r="R3" s="2">
+        <v>-1</v>
+      </c>
       <c r="S3" s="2">
         <v>1</v>
-      </c>
-      <c r="Y3" s="3"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="Y4" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -768,39 +765,39 @@
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the dialogue response selection with mouse and gamepad
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterQuest.xlsx
+++ b/Assets/Data/Excel/MasterQuest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2D8AF1-5142-47C0-B096-28C5D75A3696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0748C1BC-B87F-4890-897C-C7CE3C0AC124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -55,9 +55,6 @@
     <t>An unknown presence..</t>
   </si>
   <si>
-    <t>Scavenge for coins.</t>
-  </si>
-  <si>
     <t>Economic hardship</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>rewardKey01</t>
   </si>
   <si>
-    <t>Purchase Amulet from the vending machine</t>
-  </si>
-  <si>
     <t>Use</t>
   </si>
   <si>
@@ -164,6 +158,18 @@
   </si>
   <si>
     <t>title is not being used since it will get localized in the MasterLocalization</t>
+  </si>
+  <si>
+    <t>Scavenge for old keys.</t>
+  </si>
+  <si>
+    <t>Use old key</t>
+  </si>
+  <si>
+    <t>The response index starts from 0. If there are multiple instances of selection, the response index continues to increase.</t>
+  </si>
+  <si>
+    <t>Ex: 1st instance with 5 responses, 2nd instance with 3 responses. To get the 2nd instance of index 2(last answer), the index would be 7.</t>
   </si>
 </sst>
 </file>
@@ -579,14 +585,14 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C8:C9"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
@@ -594,7 +600,7 @@
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.21875" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -618,70 +624,70 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" t="s">
         <v>22</v>
-      </c>
-      <c r="S1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" t="s">
-        <v>24</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -689,7 +695,7 @@
         <v>20000</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -704,13 +710,13 @@
         <v>4</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I2" s="2">
         <v>2</v>
       </c>
       <c r="J2" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S2" s="2">
         <v>-1</v>
@@ -724,10 +730,10 @@
         <v>25000</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -736,25 +742,25 @@
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I3" s="2">
-        <v>10304</v>
+        <v>10201</v>
       </c>
       <c r="J3" s="2">
         <v>2</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M3" s="2">
-        <v>10304</v>
+        <v>10201</v>
       </c>
       <c r="N3" s="2">
         <v>2</v>
@@ -777,17 +783,17 @@
   <dimension ref="B2:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:K2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -804,10 +810,10 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -824,10 +830,10 @@
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -844,17 +850,47 @@
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>